<commit_message>
Final app added, audit updated
</commit_message>
<xml_diff>
--- a/Codebook - Full Audit.xlsx
+++ b/Codebook - Full Audit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="19530" windowHeight="7620"/>
+    <workbookView xWindow="5835" yWindow="0" windowWidth="19530" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="172">
   <si>
     <t>Indicator</t>
   </si>
@@ -482,10 +482,6 @@
 note max and min are based on tie in to wage</t>
   </si>
   <si>
-    <t>* Imputation question - how do they select the cities to average for imputation?
-* not balanced for population? Using absolute value?</t>
-  </si>
-  <si>
     <t>Wrong equation? Check how it is derived.</t>
   </si>
   <si>
@@ -571,9 +567,6 @@
     <t>0 again</t>
   </si>
   <si>
-    <t>Figure this out?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Entered 18, as per the note. </t>
   </si>
   <si>
@@ -581,6 +574,18 @@
   </si>
   <si>
     <t>manila? Negative lowest?</t>
+  </si>
+  <si>
+    <t>manila, tehran is 0</t>
+  </si>
+  <si>
+    <t>lima and others is 0</t>
+  </si>
+  <si>
+    <t>Should be by population</t>
+  </si>
+  <si>
+    <t>Should be per capita</t>
   </si>
 </sst>
 </file>
@@ -994,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G101"/>
+  <dimension ref="B1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,7 +1060,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -1064,13 +1069,13 @@
         <v>124</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>126</v>
@@ -1230,7 +1235,7 @@
         <v>123</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -1320,7 +1325,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>26</v>
       </c>
@@ -1334,10 +1339,10 @@
         <v>129</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="3" t="s">
         <v>2</v>
@@ -1349,10 +1354,10 @@
         <v>129</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="3" t="s">
         <v>27</v>
@@ -1364,7 +1369,7 @@
         <v>129</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -1379,10 +1384,10 @@
         <v>129</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="3" t="s">
         <v>28</v>
@@ -1394,7 +1399,7 @@
         <v>129</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -1409,7 +1414,7 @@
         <v>129</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -1450,7 +1455,7 @@
         <v>125</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -1471,13 +1476,13 @@
         <v>35</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="35" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -1510,10 +1515,10 @@
         <v>38</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -1542,7 +1547,7 @@
         <v>129</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -1557,7 +1562,7 @@
         <v>129</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -1569,10 +1574,10 @@
         <v>123</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -1601,7 +1606,7 @@
         <v>129</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -1613,7 +1618,7 @@
         <v>123</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -1622,10 +1627,10 @@
         <v>48</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -1637,10 +1642,10 @@
         <v>124</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -1655,7 +1660,7 @@
         <v>129</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="2:6" ht="60" x14ac:dyDescent="0.25">
@@ -1667,10 +1672,10 @@
         <v>124</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="2:7" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1683,11 +1688,11 @@
       <c r="D49" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="E49" s="18" t="s">
-        <v>129</v>
+      <c r="E49" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="105" x14ac:dyDescent="0.25">
@@ -1702,7 +1707,7 @@
         <v>142</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="60" x14ac:dyDescent="0.25">
@@ -1714,10 +1719,10 @@
         <v>124</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="2:7" ht="105" x14ac:dyDescent="0.25">
@@ -1726,237 +1731,238 @@
         <v>56</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
       <c r="C53" s="5" t="s">
         <v>57</v>
       </c>
+      <c r="D53" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="F53" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B54" s="8"/>
+      <c r="C54" s="9"/>
+    </row>
+    <row r="55" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B54" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E54" s="1" t="s">
+    <row r="56" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B56" s="10"/>
+      <c r="C56" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B57" s="2"/>
+      <c r="C57" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B58" s="8"/>
+      <c r="C58" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B55" s="10"/>
-      <c r="C55" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B56" s="2"/>
-      <c r="C56" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D56" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B57" s="8"/>
-      <c r="C57" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B58" s="13"/>
-      <c r="C58" s="14" t="s">
+    </row>
+    <row r="59" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B59" s="13"/>
+      <c r="C59" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D58" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B59" s="2" t="s">
+      <c r="D59" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B60" s="2"/>
-      <c r="C60" s="3" t="s">
+      <c r="D60" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B61" s="2"/>
+      <c r="C61" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D60" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B61" s="4"/>
-      <c r="C61" s="5" t="s">
+      <c r="D61" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B62" s="4"/>
+      <c r="C62" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D61" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B62" s="2" t="s">
+      <c r="D62" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B63" s="2"/>
-      <c r="C63" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="D63" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>125</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>130</v>
+        <v>69</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="65" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>130</v>
+        <v>70</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>123</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>129</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B67" s="2"/>
+      <c r="C67" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B67" s="4"/>
-      <c r="C67" s="5" t="s">
+      <c r="D67" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B68" s="4"/>
+      <c r="C68" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B68" s="2" t="s">
+      <c r="D68" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B69" s="2"/>
-      <c r="C69" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="D69" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>129</v>
@@ -1965,10 +1971,10 @@
     <row r="70" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>129</v>
@@ -1977,10 +1983,10 @@
     <row r="71" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
       <c r="C71" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>129</v>
@@ -1989,19 +1995,19 @@
     <row r="72" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
       <c r="C72" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B73" s="2"/>
+      <c r="C73" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B73" s="4"/>
-      <c r="C73" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>130</v>
@@ -2011,47 +2017,47 @@
       </c>
     </row>
     <row r="74" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="4"/>
+      <c r="C74" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B75" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="B75" s="2"/>
-      <c r="C75" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="D75" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B76" s="2"/>
       <c r="C76" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
       <c r="C77" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>123</v>
@@ -2063,177 +2069,327 @@
     <row r="78" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
       <c r="C78" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B79" s="2"/>
+      <c r="C79" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F78" s="1" t="s">
+      <c r="D79" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B80" s="4"/>
+      <c r="C80" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B82" s="4"/>
+      <c r="C82" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="79" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B79" s="4"/>
-      <c r="C79" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B80" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B81" s="4"/>
-      <c r="C81" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B82" s="15" t="s">
+    <row r="83" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B83" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C83" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="D83" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="83" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B83" s="2" t="s">
+    <row r="84" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B84" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="84" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B84" s="2"/>
-      <c r="C84" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D84" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B85" s="2"/>
       <c r="C85" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="B86" s="2"/>
+      <c r="C86" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="86" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B86" s="4"/>
-      <c r="C86" s="5" t="s">
+      <c r="D86" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="B87" s="4"/>
+      <c r="C87" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="87" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B87" s="2" t="s">
+      <c r="D87" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B88" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="88" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B88" s="2"/>
-      <c r="C88" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D88" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B89" s="2"/>
       <c r="C89" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B90" s="2"/>
+      <c r="C90" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="90" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B90" s="11" t="s">
+      <c r="D90" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B91" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C90" s="12" t="s">
+      <c r="C91" s="12" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="91" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B91" s="2"/>
-      <c r="C91" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D91" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B92" s="2"/>
       <c r="C92" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="93" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B93" s="2"/>
       <c r="C93" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D93" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E93" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B94" s="2"/>
+      <c r="C94" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="94" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B94" s="4"/>
-      <c r="C94" s="5" t="s">
+      <c r="D94" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E94" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B95" s="4"/>
+      <c r="C95" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="95" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B95" s="2" t="s">
+      <c r="D95" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E95" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B96" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="96" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B96" s="2"/>
-      <c r="C96" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D96" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B97" s="2"/>
       <c r="C97" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B98" s="2"/>
+      <c r="C98" s="3" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="98" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B98" s="4"/>
-      <c r="C98" s="5" t="s">
+      <c r="D98" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="B99" s="4"/>
+      <c r="C99" s="5" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="99" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B99" s="16" t="s">
+      <c r="D99" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B100" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="C100" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="100" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B100" s="2"/>
-      <c r="C100" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D100" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B101" s="2"/>
       <c r="C101" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B102" s="2"/>
+      <c r="C102" s="3" t="s">
         <v>116</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>